<commit_message>
added jenkins.sh for build and updated run files
</commit_message>
<xml_diff>
--- a/Automation/runs/ops_web_run.xlsx
+++ b/Automation/runs/ops_web_run.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="1240" windowWidth="28820" windowHeight="14540"/>
+    <workbookView xWindow="6260" yWindow="1240" windowWidth="28820" windowHeight="14540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>@ondemand.saucelabs.com:443/wd/hub</t>
   </si>
   <si>
-    <t>local</t>
-  </si>
-  <si>
     <t>macOS 10.12</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>remote</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -702,24 +702,24 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -761,7 +761,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -769,7 +769,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -777,7 +777,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -798,7 +798,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4" t="str">
         <f>IF(B8="QA",Configs!B2,IF(B8="DEV",Configs!B3,IF(B8="PROD",Configs!B4,"")))</f>
@@ -809,10 +809,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -841,10 +841,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -999,34 +999,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bunch of updates and fixes to ops p-0s
</commit_message>
<xml_diff>
--- a/Automation/runs/ops_web_run.xlsx
+++ b/Automation/runs/ops_web_run.xlsx
@@ -5,11 +5,11 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahanmelikyan/Documents/workspace/heal-qa-automation/Automation/runs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahanmelikyan/Documents/heal/qa-automation/Automation/runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="1240" windowWidth="28820" windowHeight="14540" activeTab="1"/>
+    <workbookView xWindow="6260" yWindow="1240" windowWidth="28820" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>Execute</t>
   </si>
@@ -162,7 +162,25 @@
     <t>Y</t>
   </si>
   <si>
-    <t>remote</t>
+    <t>local</t>
+  </si>
+  <si>
+    <t>ops.web.tests.VisitDetailsModalTest</t>
+  </si>
+  <si>
+    <t>changeProviderManualTimeSet</t>
+  </si>
+  <si>
+    <t>startVisit</t>
+  </si>
+  <si>
+    <t>endVisit</t>
+  </si>
+  <si>
+    <t>editVisitSymptoms</t>
+  </si>
+  <si>
+    <t>refundVisitTotal</t>
   </si>
 </sst>
 </file>
@@ -665,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -722,6 +740,61 @@
         <v>35</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:F6">
     <sortCondition ref="B2:B6"/>
@@ -736,7 +809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
removed some test cases from the run
</commit_message>
<xml_diff>
--- a/Automation/runs/ops_web_run.xlsx
+++ b/Automation/runs/ops_web_run.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="1240" windowWidth="28820" windowHeight="14540" activeTab="1"/>
+    <workbookView xWindow="6260" yWindow="1240" windowWidth="28820" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Execute</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>remote</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -685,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -742,7 +745,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -753,7 +756,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
@@ -764,7 +767,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
@@ -775,7 +778,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
@@ -786,7 +789,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
@@ -809,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>